<commit_message>
Added a School Timetable Lua Script and Template
</commit_message>
<xml_diff>
--- a/examples/eop_config/spreadsheets/example-timetable_schools.xlsx
+++ b/examples/eop_config/spreadsheets/example-timetable_schools.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\examples\eop_config\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495E877B-7C52-49CB-A352-B89AA4B664B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46C3304-4A81-449B-B1B8-1D67563CC56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" activeTab="2" xr2:uid="{41FF037C-E733-4109-8018-268BF2C7ACEB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" activeTab="3" xr2:uid="{41FF037C-E733-4109-8018-268BF2C7ACEB}"/>
   </bookViews>
   <sheets>
     <sheet name="district" sheetId="1" r:id="rId1"/>
@@ -1591,10 +1591,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3136,8 +3136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4E41F3-4A4C-475D-99C5-FF7DC7D3C49B}">
   <dimension ref="A1:AG195"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3235,62 +3235,62 @@
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23" t="s">
+      <c r="D3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23" t="s">
+      <c r="I3" s="24"/>
+      <c r="J3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23" t="s">
+      <c r="M3" s="24"/>
+      <c r="N3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23" t="s">
+      <c r="O3" s="24"/>
+      <c r="P3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="24" t="s">
+      <c r="Q3" s="24"/>
+      <c r="R3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="24"/>
-      <c r="T3" s="23" t="s">
+      <c r="S3" s="23"/>
+      <c r="T3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23" t="s">
+      <c r="U3" s="24"/>
+      <c r="V3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23" t="s">
+      <c r="W3" s="24"/>
+      <c r="X3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23" t="s">
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23" t="s">
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23" t="s">
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="AE3" s="23"/>
+      <c r="AE3" s="24"/>
     </row>
     <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
@@ -15229,6 +15229,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="A1:AE1"/>
     <mergeCell ref="A2:A4"/>
@@ -15242,12 +15248,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -15258,7 +15258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614FD235-4236-4207-9A64-880D49E7EAB5}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -15459,7 +15459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B013458-3FFF-4982-A44F-299B41089B86}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -16035,62 +16035,62 @@
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23" t="s">
+      <c r="D3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23" t="s">
+      <c r="I3" s="24"/>
+      <c r="J3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23" t="s">
+      <c r="M3" s="24"/>
+      <c r="N3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23" t="s">
+      <c r="O3" s="24"/>
+      <c r="P3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23" t="s">
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23" t="s">
+      <c r="S3" s="24"/>
+      <c r="T3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23" t="s">
+      <c r="U3" s="24"/>
+      <c r="V3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23" t="s">
+      <c r="W3" s="24"/>
+      <c r="X3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23" t="s">
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23" t="s">
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23" t="s">
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="AE3" s="23"/>
+      <c r="AE3" s="24"/>
     </row>
     <row r="4" spans="1:32" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
@@ -17399,6 +17399,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="A1:AE1"/>
     <mergeCell ref="A2:A4"/>
@@ -17412,12 +17418,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>